<commit_message>
heatsink, weight distribution updates
</commit_message>
<xml_diff>
--- a/FE12/Weight Distribution Studies/Accumulator Weight Distribution.xlsx
+++ b/FE12/Weight Distribution Studies/Accumulator Weight Distribution.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laptop\OneDrive - University of California, Davis\Documents\GitHub\FE12-Accumulator\FE12\Weight Distribution Studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D68762F-F9C9-4726-8658-9F90487EFA4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BD9EDF-DBDB-4034-AF5E-36552FCC20EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{879E6154-3167-41E1-8BFC-E61D3D520CD3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{879E6154-3167-41E1-8BFC-E61D3D520CD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="98">
   <si>
     <t>Subpack</t>
   </si>
@@ -92,9 +92,6 @@
     <t>Lid</t>
   </si>
   <si>
-    <t>Mounts and Gussets</t>
-  </si>
-  <si>
     <t>Insulating Sheet</t>
   </si>
   <si>
@@ -257,9 +254,6 @@
     <t>PE floor (fans)</t>
   </si>
   <si>
-    <t>flat sheet without cutouts or flanges yet</t>
-  </si>
-  <si>
     <t>smaller for FE12, estimate for now</t>
   </si>
   <si>
@@ -269,12 +263,6 @@
     <t xml:space="preserve">Mounts </t>
   </si>
   <si>
-    <t>CAD, get weight, steel</t>
-  </si>
-  <si>
-    <t>get FE11 weight, estimate a bit smaller</t>
-  </si>
-  <si>
     <t>FE12 % of weight</t>
   </si>
   <si>
@@ -299,9 +287,6 @@
     <t>Difference</t>
   </si>
   <si>
-    <t>20% goal</t>
-  </si>
-  <si>
     <t>Volume of FE12</t>
   </si>
   <si>
@@ -329,7 +314,22 @@
     <t>in2</t>
   </si>
   <si>
-    <t>volume goal 25%</t>
+    <t>with first draft cutouts</t>
+  </si>
+  <si>
+    <t>add air duct weight</t>
+  </si>
+  <si>
+    <t>Ratio</t>
+  </si>
+  <si>
+    <t>Total FE11 Actual Weight</t>
+  </si>
+  <si>
+    <t>volume goal</t>
+  </si>
+  <si>
+    <t>mass goal</t>
   </si>
 </sst>
 </file>
@@ -354,13 +354,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -388,12 +387,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -436,7 +429,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -447,7 +440,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1168,10 +1164,10 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>16.45</c:v>
+                  <c:v>15.339072</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.36</c:v>
+                  <c:v>0.24907199999999999</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
                   <c:v>0.69899999999999995</c:v>
@@ -1183,7 +1179,7 @@
                   <c:v>2.0914000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="General">
-                  <c:v>0.82260000000000133</c:v>
+                  <c:v>1.933527999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1877,10 +1873,10 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>16.45</c:v>
+                  <c:v>15.339072</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.36</c:v>
+                  <c:v>0.24907199999999999</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
                   <c:v>0.69899999999999995</c:v>
@@ -1892,7 +1888,7 @@
                   <c:v>2.0914000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="General">
-                  <c:v>0.82260000000000133</c:v>
+                  <c:v>1.933527999999999</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="General">
                   <c:v>47.1</c:v>
@@ -4242,15 +4238,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
+      <xdr:colOff>561974</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:rowOff>56029</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>261257</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>65314</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>380999</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>123265</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4278,15 +4274,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>304801</xdr:colOff>
+      <xdr:colOff>237565</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:rowOff>134470</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>119743</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>119742</xdr:rowOff>
+      <xdr:colOff>1176617</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>164565</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4314,15 +4310,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>582490</xdr:colOff>
+      <xdr:colOff>579100</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>130053</xdr:rowOff>
+      <xdr:rowOff>145676</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>506290</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>154818</xdr:rowOff>
+      <xdr:colOff>392205</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>44823</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4350,15 +4346,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>371474</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>57149</xdr:rowOff>
+      <xdr:colOff>248209</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>56030</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>344365</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>73269</xdr:rowOff>
+      <xdr:colOff>168088</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>78441</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4705,67 +4701,67 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3F21477-A8EC-4562-AE62-81692505D30C}">
   <dimension ref="A1:Q70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="K2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="L2" t="s">
+        <v>69</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="O2" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="M2" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>71</v>
-      </c>
       <c r="P2" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -4784,7 +4780,7 @@
         <v>67.510000000000005</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K3" s="1">
         <f>B3</f>
@@ -4794,11 +4790,11 @@
         <v>5.04</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N3" s="1">
         <f>SUM(E3:E8)</f>
-        <v>16.45</v>
+        <v>15.339072</v>
       </c>
       <c r="O3">
         <v>8</v>
@@ -4811,7 +4807,7 @@
         <v>31.176000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -4825,7 +4821,7 @@
         <v>3.63</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K4" s="1">
         <f>SUM(B5:B15)</f>
@@ -4835,24 +4831,24 @@
         <v>1.5</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N4" s="6">
         <f>E8</f>
-        <v>1.36</v>
+        <v>0.24907199999999999</v>
       </c>
       <c r="O4">
         <v>1.36</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q4" s="1">
         <f>G3-Q3</f>
         <v>36.334000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -4860,16 +4856,16 @@
         <v>0.05</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5" s="1">
         <v>1.95</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K5" s="1">
         <f>SUM(B16:B17)</f>
@@ -4879,7 +4875,7 @@
         <v>3.9E-2</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N5" s="1">
         <f>SUM(E14:E21)</f>
@@ -4889,7 +4885,7 @@
         <v>0.69899999999999995</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
@@ -4898,7 +4894,7 @@
         <v>0.06</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E6" s="1">
         <f>0.58*4</f>
@@ -4908,7 +4904,7 @@
         <v>67.900000000000006</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K6" s="1">
         <f>SUM(B18:B19)</f>
@@ -4918,7 +4914,7 @@
         <v>0.1</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N6" s="1">
         <f>SUM(E21:E28)</f>
@@ -4928,7 +4924,7 @@
         <v>0.42699999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -4936,7 +4932,7 @@
         <v>0.05</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" s="1">
         <f>0.45</f>
@@ -4953,7 +4949,7 @@
         <v>0.13</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N7" s="1">
         <f>SUM(E9:E13)+SUM(E29:E30)</f>
@@ -4963,7 +4959,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -4971,20 +4967,21 @@
         <v>0.05</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="E8" s="9">
-        <v>1.36</v>
+        <f>4*0.02278+4*0.023676+2*0.031624</f>
+        <v>0.24907199999999999</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H8" s="2">
         <f>G3-67.9</f>
         <v>-0.39000000000000057</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K8" s="1">
         <f>B21</f>
@@ -4994,17 +4991,17 @@
         <v>0.35</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N8" s="1">
         <f>E32</f>
-        <v>0.82260000000000133</v>
+        <v>1.933527999999999</v>
       </c>
       <c r="O8">
         <v>0.6</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -5013,13 +5010,13 @@
         <v>0.08</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E9" s="1">
         <v>0.79</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H9" s="2">
         <f>G3-67.51</f>
@@ -5034,7 +5031,7 @@
         <v>7.1589999999999989</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N9" s="1">
         <f>4.71*10</f>
@@ -5045,16 +5042,16 @@
         <v>35.794999999999995</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" s="1">
         <f>2*0.02</f>
         <v>0.04</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E10" s="1">
         <f>0.03*20</f>
@@ -5070,30 +5067,30 @@
       </c>
       <c r="N10">
         <f>SUM(N3:N9)</f>
-        <v>68.95</v>
+        <v>67.839072000000002</v>
       </c>
       <c r="O10">
         <f>SUM(O3:O9)</f>
         <v>48.380999999999993</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="1">
         <f>2*0.03</f>
         <v>0.06</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E11" s="1">
         <f>0.00907*20</f>
         <v>0.18140000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -5101,14 +5098,14 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E12" s="1">
         <f>0.04*3</f>
         <v>0.12</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -5116,14 +5113,14 @@
         <v>0.16</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E13" s="1">
         <f>0.01*5</f>
         <v>0.05</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
@@ -5131,13 +5128,13 @@
         <v>0.18</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E14" s="1">
         <v>0.03</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -5146,14 +5143,14 @@
         <v>0.02</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E15" s="1">
         <f>0.059</f>
         <v>5.8999999999999997E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -5161,89 +5158,89 @@
         <v>1.9E-2</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E16" s="1">
         <f>2*0.19</f>
         <v>0.38</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B17" s="1">
         <f>0.02</f>
         <v>0.02</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E17" s="1">
         <v>0.02</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B18" s="1">
         <f>5.88/1000*11</f>
         <v>6.4680000000000001E-2</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E18" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="1">
         <f>2*0.01</f>
         <v>0.02</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E19" s="1">
         <v>0.01</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20" s="4">
         <f>SUM(B3:B19)</f>
         <v>4.3912799999999983</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E20" s="1">
         <v>0.02</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B21" s="4">
         <f>B22-B20</f>
         <v>0.31872000000000167</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E21" s="1">
         <v>0.08</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>14</v>
       </c>
@@ -5251,162 +5248,167 @@
         <v>4.71</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E22" s="1">
         <v>0.02</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D23" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E23" s="1">
         <v>0.16</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B24">
-        <f>6.44+B30+B21</f>
-        <v>6.9177200000000019</v>
+        <f>6.65+B30+B21</f>
+        <v>7.1277200000000018</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E24" s="1">
         <f>0.03</f>
         <v>0.03</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B25">
         <f>B24/B22</f>
-        <v>1.4687303609341831</v>
+        <v>1.5133163481953296</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E25" s="1">
         <v>0.01</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D26" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E26" s="1">
         <f>2*(0.01)</f>
         <v>0.02</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B27">
         <f>B24*5</f>
-        <v>34.588600000000007</v>
+        <v>35.638600000000011</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E27" s="1">
         <f>2*0.01</f>
         <v>0.02</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B28">
         <f>B27/47.1</f>
-        <v>0.73436518046709143</v>
+        <v>0.75665817409766478</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E28" s="1">
         <f>0.027+0.06</f>
         <v>8.6999999999999994E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D29" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E29" s="1">
         <f>0.03+0.01</f>
         <v>0.04</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B30">
         <f>0.053*3</f>
         <v>0.159</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E30" s="1">
         <v>0.31</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B31">
         <f>B30*5</f>
         <v>0.79500000000000004</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E31" s="4">
         <f>SUM(E2:E30)</f>
-        <v>19.587400000000002</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+        <v>18.476472000000005</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D32" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E32" s="4">
         <f>67.51-B22*10-E31</f>
-        <v>0.82260000000000133</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1.933527999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D33" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E33" s="3">
         <f>E31+E32</f>
         <v>20.410000000000004</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E41" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>16</v>
       </c>
@@ -5416,359 +5418,371 @@
       </c>
       <c r="E42">
         <f>B70/E33</f>
-        <v>0.72007349338559501</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
+        <v>0.74442038216560469</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B43" s="1">
-        <v>2</v>
-      </c>
-      <c r="C43" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.4193199999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B44" s="1">
-        <v>1.06</v>
+        <v>1.5376000000000001</v>
       </c>
       <c r="C44" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B45" s="1">
         <f>0.583*5</f>
         <v>2.915</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
-        <v>76</v>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="s">
+        <v>74</v>
       </c>
       <c r="B46" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="C46" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B47" s="1">
         <f>0.03*10</f>
         <v>0.3</v>
       </c>
       <c r="C47" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B48" s="1">
         <f>0.00907*10</f>
         <v>9.0700000000000003E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B49" s="1">
         <v>0.04</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B50" s="1">
         <f>0.01*8</f>
         <v>0.08</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B51" s="1">
         <v>0.03</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B52" s="1">
         <f>0.059</f>
         <v>5.8999999999999997E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B53" s="1">
         <f>2*0.19</f>
         <v>0.38</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B54" s="1">
         <v>0.02</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B55" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B56" s="1">
         <v>0.01</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B57" s="1">
         <v>0.02</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B58" s="1">
         <v>0.08</v>
       </c>
-      <c r="J58" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B59" s="1">
         <v>0.02</v>
       </c>
-      <c r="D59" t="s">
-        <v>88</v>
-      </c>
-      <c r="G59" t="s">
-        <v>92</v>
-      </c>
-      <c r="J59">
-        <f>E63/H63</f>
-        <v>0.57514665286404409</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D59" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J59" t="s">
+        <v>89</v>
+      </c>
+      <c r="K59" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B60" s="1">
         <v>0.16</v>
       </c>
-      <c r="D60" t="s">
-        <v>90</v>
-      </c>
-      <c r="E60">
+      <c r="D60" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E60" s="1">
         <f>22</f>
         <v>22</v>
       </c>
-      <c r="G60" t="s">
-        <v>93</v>
-      </c>
-      <c r="H60">
+      <c r="G60" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H60" s="1">
         <v>27.6</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J60">
+        <f>E63/H63</f>
+        <v>0.53289270405496503</v>
+      </c>
+      <c r="K60" s="12">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B61" s="1">
         <f>0.03</f>
         <v>0.03</v>
       </c>
-      <c r="D61" t="s">
-        <v>89</v>
-      </c>
-      <c r="E61">
-        <f>14.5</f>
-        <v>14.5</v>
-      </c>
-      <c r="G61" t="s">
-        <v>89</v>
-      </c>
-      <c r="H61">
+      <c r="D61" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E61" s="1">
+        <v>14.514272</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H61" s="1">
         <v>21</v>
       </c>
       <c r="J61" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B62" s="1">
         <v>0.01</v>
       </c>
-      <c r="D62" t="s">
-        <v>91</v>
-      </c>
-      <c r="E62">
-        <f>9.28+0.125</f>
-        <v>9.4049999999999994</v>
-      </c>
-      <c r="G62" t="s">
-        <v>91</v>
-      </c>
-      <c r="H62">
+      <c r="D62" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E62" s="1">
+        <v>8.7054799999999997</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H62" s="1">
         <v>9</v>
       </c>
       <c r="J62">
         <f>H63-E63</f>
-        <v>2216.2050000000008</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+        <v>2436.6184985676805</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B63" s="1">
         <f>2*(0.01)</f>
         <v>0.02</v>
       </c>
-      <c r="D63" t="s">
-        <v>88</v>
-      </c>
-      <c r="E63">
+      <c r="D63" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E63" s="1">
         <f>E60*E61*E62</f>
-        <v>3000.1949999999997</v>
-      </c>
-      <c r="F63" t="s">
-        <v>96</v>
-      </c>
-      <c r="G63" t="s">
-        <v>92</v>
-      </c>
-      <c r="H63">
+        <v>2779.7815014323201</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H63" s="1">
         <f>H60*H61*H62</f>
         <v>5216.4000000000005</v>
       </c>
-      <c r="I63" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B64" s="1">
         <f>2*0.01</f>
         <v>0.02</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F64" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B65" s="1">
         <f>0.027+0.06</f>
         <v>8.6999999999999994E-2</v>
       </c>
       <c r="D65" t="s">
-        <v>85</v>
-      </c>
-      <c r="E65">
-        <f>B70+B27</f>
-        <v>49.285300000000007</v>
-      </c>
-      <c r="F65">
-        <f>E65/67.9</f>
-        <v>0.72585125184094257</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="E65" s="13">
+        <f>G6</f>
+        <v>67.900000000000006</v>
+      </c>
+      <c r="F65" s="13"/>
       <c r="G65" t="s">
-        <v>87</v>
-      </c>
-      <c r="H65" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B66" s="1">
         <f>0.03+0.01</f>
         <v>0.04</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D66" t="s">
+        <v>81</v>
+      </c>
+      <c r="E66" s="11">
+        <f>B70+B27</f>
+        <v>50.832220000000007</v>
+      </c>
+      <c r="F66" s="11">
+        <f>E66/E65</f>
+        <v>0.74863357879234171</v>
+      </c>
+      <c r="G66" s="12">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B67" s="1">
         <v>0.31</v>
       </c>
       <c r="E67" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B68" s="4">
         <f>SUM(B42:B67)</f>
-        <v>13.696699999999996</v>
-      </c>
-      <c r="E68">
-        <f>67.9-E65</f>
-        <v>18.614699999999999</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+        <v>14.193619999999994</v>
+      </c>
+      <c r="E68" s="11">
+        <f>E65-E66</f>
+        <v>17.067779999999999</v>
+      </c>
+      <c r="F68" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B69" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B70" s="3">
         <f>B68+B69</f>
-        <v>14.696699999999996</v>
+        <v>15.193619999999994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
weight distribution spreadsheet update
</commit_message>
<xml_diff>
--- a/FE12/Weight Distribution Studies/Accumulator Weight Distribution.xlsx
+++ b/FE12/Weight Distribution Studies/Accumulator Weight Distribution.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laptop\OneDrive - University of California, Davis\Documents\GitHub\FE12-Accumulator\FE12\Weight Distribution Studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7963963-8863-44AB-A256-1D6C59A2696C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C191ABCE-1C37-478C-B48D-3670312E7312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{879E6154-3167-41E1-8BFC-E61D3D520CD3}"/>
   </bookViews>
@@ -489,7 +489,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,7 +585,6 @@
           <c:dPt>
             <c:idx val="1"/>
             <c:bubble3D val="0"/>
-            <c:spPr/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000001C-4BA5-44F5-AE35-4BE3B0C01E6D}"/>
@@ -595,7 +594,6 @@
           <c:dPt>
             <c:idx val="2"/>
             <c:bubble3D val="0"/>
-            <c:spPr/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000001D-4BA5-44F5-AE35-4BE3B0C01E6D}"/>
@@ -605,7 +603,6 @@
           <c:dPt>
             <c:idx val="3"/>
             <c:bubble3D val="0"/>
-            <c:spPr/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000001E-4BA5-44F5-AE35-4BE3B0C01E6D}"/>
@@ -615,7 +612,6 @@
           <c:dPt>
             <c:idx val="4"/>
             <c:bubble3D val="0"/>
-            <c:spPr/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000001F-4BA5-44F5-AE35-4BE3B0C01E6D}"/>
@@ -625,7 +621,6 @@
           <c:dPt>
             <c:idx val="5"/>
             <c:bubble3D val="0"/>
-            <c:spPr/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000020-4BA5-44F5-AE35-4BE3B0C01E6D}"/>
@@ -1095,7 +1090,6 @@
           <c:dPt>
             <c:idx val="1"/>
             <c:bubble3D val="0"/>
-            <c:spPr/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000001C-3D62-4C71-9E77-F8EEE9F04FE1}"/>
@@ -1105,7 +1099,6 @@
           <c:dPt>
             <c:idx val="2"/>
             <c:bubble3D val="0"/>
-            <c:spPr/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000001D-3D62-4C71-9E77-F8EEE9F04FE1}"/>
@@ -1115,7 +1108,6 @@
           <c:dPt>
             <c:idx val="3"/>
             <c:bubble3D val="0"/>
-            <c:spPr/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000001E-3D62-4C71-9E77-F8EEE9F04FE1}"/>
@@ -1125,7 +1117,6 @@
           <c:dPt>
             <c:idx val="4"/>
             <c:bubble3D val="0"/>
-            <c:spPr/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000001F-3D62-4C71-9E77-F8EEE9F04FE1}"/>
@@ -1135,7 +1126,6 @@
           <c:dPt>
             <c:idx val="5"/>
             <c:bubble3D val="0"/>
-            <c:spPr/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000020-3D62-4C71-9E77-F8EEE9F04FE1}"/>
@@ -2777,7 +2767,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>FE11 Accumulator</a:t>
+              <a:t>FE12 Accumulator</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -3672,6 +3662,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-8D9D-4BC4-9C18-85D43D05E6E6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -3687,6 +3682,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-8D9D-4BC4-9C18-85D43D05E6E6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -3702,6 +3702,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-8D9D-4BC4-9C18-85D43D05E6E6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -3717,6 +3722,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-8D9D-4BC4-9C18-85D43D05E6E6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -3732,6 +3742,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-8D9D-4BC4-9C18-85D43D05E6E6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -3749,6 +3764,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-8D9D-4BC4-9C18-85D43D05E6E6}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -7962,8 +7982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3F21477-A8EC-4562-AE62-81692505D30C}">
   <dimension ref="A1:Q92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I92" sqref="I92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>